<commit_message>
Subject Excels complete. Beginning AI soon.
</commit_message>
<xml_diff>
--- a/Subject2_Data.xlsx
+++ b/Subject2_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevo\source\repos\RFID_Deployment_Nightly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C9F196-F02F-4806-9ADD-4A3A9149707B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594F45F5-BCE8-4FB6-960F-803EFF6E255D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -120,7 +120,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -206,19 +206,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -526,7 +526,7 @@
   <dimension ref="A1:O354"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P300" sqref="P300"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -577,10 +577,10 @@
         <v>27</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.45">
@@ -14405,22 +14405,22 @@
       <c r="A296" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B296" s="6" t="s">
+      <c r="B296" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C296" s="5"/>
-      <c r="D296" s="5"/>
-      <c r="E296" s="5"/>
-      <c r="F296" s="5"/>
-      <c r="G296" s="5"/>
-      <c r="H296" s="5"/>
-      <c r="I296" s="5"/>
-      <c r="J296" s="5"/>
-      <c r="K296" s="5"/>
-      <c r="L296" s="5"/>
-      <c r="M296" s="5"/>
-      <c r="N296" s="5"/>
-      <c r="O296" s="5"/>
+      <c r="C296" s="6"/>
+      <c r="D296" s="6"/>
+      <c r="E296" s="6"/>
+      <c r="F296" s="6"/>
+      <c r="G296" s="6"/>
+      <c r="H296" s="6"/>
+      <c r="I296" s="6"/>
+      <c r="J296" s="6"/>
+      <c r="K296" s="6"/>
+      <c r="L296" s="6"/>
+      <c r="M296" s="6"/>
+      <c r="N296" s="6"/>
+      <c r="O296" s="6"/>
     </row>
     <row r="297" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A297" s="2">

</xml_diff>